<commit_message>
April 2021 Repository update
</commit_message>
<xml_diff>
--- a/IRSE/acq/irse_acq_info.xlsx
+++ b/IRSE/acq/irse_acq_info.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tongg\PycharmProjects\mr-sequence-validation\packaged_sequences\IRSE\acq\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tongg\Documents\Research\Manuscripts\seq_validation\Revision_1_additions\Repository\mr-sequence-validation-main_updated\IRSE\acq\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5468B67-E221-48A3-8C28-2A41C15F26BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1F4CDDA-4F4E-4402-9CD8-5133CB1CEF28}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="11949" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="11949" xr2:uid="{46B9FD32-6038-4DBD-9203-1FE6CFECBD36}"/>
   </bookViews>
   <sheets>
-    <sheet name="Acquisitions" sheetId="1" r:id="rId1"/>
+    <sheet name="Apr 2021" sheetId="11" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,9 +25,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
-  <si>
-    <t>90/180</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
+  <si>
+    <t>Date</t>
   </si>
   <si>
     <t>FID</t>
@@ -39,81 +39,61 @@
     <t>Description</t>
   </si>
   <si>
-    <t>TI (ms)</t>
-  </si>
-  <si>
     <t>FA (deg)</t>
   </si>
   <si>
+    <t>TR(ms)</t>
+  </si>
+  <si>
+    <t>FOV(mm)</t>
+  </si>
+  <si>
+    <t>Thk(mm)</t>
+  </si>
+  <si>
+    <t>TE(ms)</t>
+  </si>
+  <si>
+    <t>TI(ms)</t>
+  </si>
+  <si>
     <t>Phantom</t>
   </si>
   <si>
-    <t>n_slices</t>
-  </si>
-  <si>
-    <t>FOV(mm)</t>
-  </si>
-  <si>
-    <t>Thk(mm)</t>
-  </si>
-  <si>
-    <t>TR(ms)</t>
-  </si>
-  <si>
-    <t>TE(ms)</t>
-  </si>
-  <si>
-    <t>Read</t>
-  </si>
-  <si>
-    <t>Phase</t>
-  </si>
-  <si>
-    <t>Slice</t>
-  </si>
-  <si>
-    <t>x</t>
-  </si>
-  <si>
-    <t>z</t>
-  </si>
-  <si>
-    <t>Slice loc (mm)</t>
-  </si>
-  <si>
-    <t># Channels</t>
+    <t>ACR</t>
+  </si>
+  <si>
+    <t>Coil</t>
+  </si>
+  <si>
+    <t>System</t>
   </si>
   <si>
     <t>N</t>
   </si>
   <si>
-    <t xml:space="preserve">ACR </t>
-  </si>
-  <si>
-    <t>y</t>
-  </si>
-  <si>
-    <t>Slice Gap</t>
-  </si>
-  <si>
-    <t>Pht. Placement</t>
-  </si>
-  <si>
-    <t>z=0 at "nose"</t>
-  </si>
-  <si>
-    <t>IRSE ACR Slices (rep. 1)</t>
-  </si>
-  <si>
-    <t>IRSE ACR Slices (rep. 2)</t>
+    <t>Head 20</t>
+  </si>
+  <si>
+    <t>PyPulseq IRSE - ACR Slices - Rep 1</t>
+  </si>
+  <si>
+    <t>PyPulseq IRSE - ACR Slices - Rep 2</t>
+  </si>
+  <si>
+    <t>Siemens Magnetom Prisma 3T</t>
+  </si>
+  <si>
+    <t>Slice displacement (mm)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="\+0;\-0;0"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -131,7 +111,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -140,12 +120,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="1"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -153,27 +139,45 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF208CA6"/>
+      <color rgb="FF6B6B6B"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -202,7 +206,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -214,7 +218,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -261,6 +265,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -296,6 +317,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -447,210 +485,186 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1E8BCDD-81E9-48A3-B41E-90B677B212C0}">
+  <dimension ref="A1:V7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="2" width="9.23046875" style="2"/>
-    <col min="3" max="3" width="25.3828125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="9.84375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="12.921875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="10.69140625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="6.07421875" style="2" customWidth="1"/>
-    <col min="8" max="8" width="6.53515625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="4.765625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="8.4609375" style="2" customWidth="1"/>
-    <col min="11" max="11" width="12.69140625" style="2" customWidth="1"/>
-    <col min="12" max="12" width="8.4609375" style="2" customWidth="1"/>
-    <col min="13" max="13" width="8.3046875" style="2" customWidth="1"/>
-    <col min="14" max="14" width="4.3046875" style="2" customWidth="1"/>
-    <col min="15" max="16384" width="9.23046875" style="2"/>
+    <col min="1" max="1" width="12.61328125" style="1" customWidth="1"/>
+    <col min="2" max="3" width="9.23046875" style="2"/>
+    <col min="4" max="4" width="29.921875" style="2" customWidth="1"/>
+    <col min="5" max="6" width="9.23046875" style="2"/>
+    <col min="7" max="7" width="30.921875" style="2" customWidth="1"/>
+    <col min="8" max="8" width="21.3828125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="6.53515625" style="2" customWidth="1"/>
+    <col min="10" max="16384" width="9.23046875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="H1" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="K1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="O1" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.4">
+      <c r="A2" s="1">
+        <v>44298</v>
+      </c>
+      <c r="B2" s="2">
+        <v>6186</v>
+      </c>
+      <c r="C2" s="2">
+        <v>827</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="E2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="2">
+        <v>-4.4000000000000004</v>
+      </c>
+      <c r="I2" s="2">
+        <v>256</v>
+      </c>
+      <c r="J2" s="2">
+        <v>250</v>
+      </c>
+      <c r="K2" s="2">
+        <v>5</v>
+      </c>
+      <c r="L2" s="2">
+        <v>2000</v>
+      </c>
+      <c r="M2" s="2">
         <v>12</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" s="1" t="s">
+      <c r="N2" s="2">
+        <v>150</v>
+      </c>
+      <c r="O2" s="2">
+        <v>90</v>
+      </c>
+      <c r="P2" s="4"/>
+      <c r="Q2" s="4"/>
+      <c r="R2" s="4"/>
+      <c r="S2" s="4"/>
+      <c r="T2" s="4"/>
+      <c r="U2" s="4"/>
+      <c r="V2" s="4"/>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.4">
+      <c r="A3" s="1">
+        <v>44298</v>
+      </c>
+      <c r="B3" s="2">
+        <v>6187</v>
+      </c>
+      <c r="C3" s="2">
+        <v>828</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="S1" s="1" t="s">
+      <c r="H3" s="2">
+        <v>-4.4000000000000004</v>
+      </c>
+      <c r="I3" s="2">
+        <v>256</v>
+      </c>
+      <c r="J3" s="2">
+        <v>250</v>
+      </c>
+      <c r="K3" s="2">
         <v>5</v>
       </c>
+      <c r="L3" s="2">
+        <v>2000</v>
+      </c>
+      <c r="M3" s="2">
+        <v>12</v>
+      </c>
+      <c r="N3" s="2">
+        <v>150</v>
+      </c>
+      <c r="O3" s="2">
+        <v>90</v>
+      </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.4">
-      <c r="A2" s="2">
-        <v>1908</v>
-      </c>
-      <c r="B2" s="2">
-        <v>546</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F2" s="2">
-        <v>20</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J2" s="2">
-        <v>11</v>
-      </c>
-      <c r="K2" s="3">
-        <v>5</v>
-      </c>
-      <c r="L2" s="2">
-        <v>5</v>
-      </c>
-      <c r="M2" s="2">
-        <v>5</v>
-      </c>
-      <c r="N2" s="2">
-        <v>256</v>
-      </c>
-      <c r="O2" s="2">
-        <v>250</v>
-      </c>
-      <c r="P2" s="2">
-        <v>2000</v>
-      </c>
-      <c r="Q2" s="2">
-        <v>12</v>
-      </c>
-      <c r="R2" s="2">
-        <v>100</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>0</v>
-      </c>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.4">
+      <c r="G6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="P6" s="3"/>
     </row>
-    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="2">
-        <v>1909</v>
-      </c>
-      <c r="B3" s="2">
-        <v>547</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F3" s="2">
-        <v>20</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J3" s="2">
-        <v>11</v>
-      </c>
-      <c r="K3" s="3">
-        <v>5</v>
-      </c>
-      <c r="L3" s="2">
-        <v>5</v>
-      </c>
-      <c r="M3" s="2">
-        <v>5</v>
-      </c>
-      <c r="N3" s="2">
-        <v>256</v>
-      </c>
-      <c r="O3" s="2">
-        <v>250</v>
-      </c>
-      <c r="P3" s="2">
-        <v>2000</v>
-      </c>
-      <c r="Q3" s="2">
-        <v>12</v>
-      </c>
-      <c r="R3" s="2">
-        <v>100</v>
-      </c>
-      <c r="S3" s="2" t="s">
-        <v>0</v>
-      </c>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.4">
+      <c r="G7" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>